<commit_message>
Added updates for latest PDFTronGo lib update.
</commit_message>
<xml_diff>
--- a/samples/TestFiles/simple-excel_2007.xlsx
+++ b/samples/TestFiles/simple-excel_2007.xlsx
@@ -17,118 +17,157 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<!--OOXMLEditor: Added index comments-->
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+  <!-- String id="0" -->
   <si>
     <t>Quantity</t>
   </si>
+  <!-- String id="1" -->
   <si>
     <t>Total</t>
   </si>
+  <!-- String id="2" -->
   <si>
     <t>Soil</t>
   </si>
+  <!-- String id="3" -->
   <si>
     <t>Seeds</t>
   </si>
+  <!-- String id="4" -->
   <si>
     <t>Plants</t>
   </si>
+  <!-- String id="5" -->
   <si>
     <t>Flowers</t>
   </si>
+  <!-- String id="6" -->
   <si>
     <t>Trees</t>
   </si>
+  <!-- String id="7" -->
   <si>
     <t>Plant Food</t>
   </si>
+  <!-- String id="8" -->
   <si>
     <t>Mulch</t>
   </si>
+  <!-- String id="9" -->
   <si>
     <t>Total Costs</t>
   </si>
+  <!-- String id="10" -->
   <si>
     <t>Difference</t>
   </si>
+  <!-- String id="11" -->
   <si>
     <t>Fertilizer/Compost</t>
   </si>
+  <!-- String id="12" -->
   <si>
     <t>Description</t>
   </si>
+  <!-- String id="13" -->
   <si>
     <t>Name</t>
   </si>
+  <!-- String id="14" -->
   <si>
     <t>Total Plants</t>
   </si>
+  <!-- String id="15" -->
   <si>
     <t>Cost Each</t>
   </si>
+  <!-- String id="16" -->
   <si>
     <t>Total Flowers</t>
   </si>
+  <!-- String id="17" -->
   <si>
     <t>Total Trees</t>
   </si>
+  <!-- String id="18" -->
   <si>
     <t>Total Seeds</t>
   </si>
+  <!-- String id="19" -->
   <si>
     <t>Total Plant Food</t>
   </si>
+  <!-- String id="20" -->
   <si>
     <t>Total Soil</t>
   </si>
+  <!-- String id="21" -->
   <si>
     <t>Total Mulch</t>
   </si>
+  <!-- String id="22" -->
   <si>
     <t>Total Fertilizer/Compost</t>
   </si>
+  <!-- String id="23" -->
   <si>
     <t>Rhododendron</t>
   </si>
+  <!-- String id="24" -->
   <si>
     <t>Petunia</t>
   </si>
+  <!-- String id="25" -->
   <si>
     <t>Annual, purple and white</t>
   </si>
+  <!-- String id="26" -->
   <si>
     <t>Furniture/Statuary</t>
   </si>
+  <!-- String id="27" -->
   <si>
     <t>Total Furniture/Statuary</t>
   </si>
+  <!-- String id="28" -->
   <si>
     <t>Fencing</t>
   </si>
+  <!-- String id="29" -->
   <si>
     <t>Total Fencing</t>
   </si>
+  <!-- String id="30" -->
   <si>
     <t>Japanese Maple</t>
   </si>
+  <!-- String id="31" -->
   <si>
     <t>Leafy tree</t>
   </si>
+  <!-- String id="32" -->
   <si>
     <t>Herbicides/Pesticides</t>
   </si>
+  <!-- String id="33" -->
   <si>
     <t>Total Herbicides/Pesticides</t>
   </si>
+  <!-- String id="34" -->
   <si>
     <t>Flowering evergreen</t>
   </si>
+  <!-- String id="35" -->
   <si>
     <t xml:space="preserve">   </t>
   </si>
+  <!-- String id="36" -->
   <si>
     <t>Budgeted amount</t>
   </si>
+  <!-- String id="37" -->
   <si>
     <t xml:space="preserve"> Garden Budget</t>
   </si>
@@ -136,21 +175,25 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
+<!--OOXMLEditor: Added index comments-->
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="13">
+    <!-- fontId="0" -->
     <font>
       <sz val="10"/>
       <name val="Arial"/>
     </font>
+    <!-- fontId="1" -->
     <font>
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <!-- fontId="2" -->
     <font>
       <b/>
       <sz val="9"/>
@@ -158,11 +201,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <!-- fontId="3" -->
     <font>
       <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <!-- fontId="4" -->
     <font>
       <b/>
       <sz val="24"/>
@@ -170,6 +215,7 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <!-- fontId="5" -->
     <font>
       <b/>
       <sz val="26"/>
@@ -177,97 +223,114 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <!-- fontId="6" -->
     <font>
       <sz val="10"/>
-      <name val="Century Gothic"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
+    <!-- fontId="7" -->
     <font>
       <b/>
       <sz val="10"/>
-      <name val="Century Gothic"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
+    <!-- fontId="8" -->
     <font>
       <b/>
       <sz val="10"/>
       <color indexed="9"/>
-      <name val="Century Gothic"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
+    <!-- fontId="9" -->
     <font>
       <sz val="10"/>
       <color indexed="9"/>
-      <name val="Century Gothic"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
+    <!-- fontId="10" -->
     <font>
       <sz val="9"/>
       <color indexed="9"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <!-- fontId="11" -->
     <font>
       <sz val="22"/>
       <color indexed="9"/>
-      <name val="Century Gothic"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
+    <!-- fontId="12" -->
     <font>
       <sz val="9"/>
-      <name val="Century Gothic"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
   <fills count="10">
+    <!-- fillId="0" -->
     <fill>
       <patternFill patternType="none"/>
     </fill>
+    <!-- fillId="1" -->
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <!-- fillId="2" -->
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="14"/>
         <bgColor indexed="24"/>
       </patternFill>
     </fill>
+    <!-- fillId="3" -->
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="63"/>
         <bgColor indexed="24"/>
       </patternFill>
     </fill>
+    <!-- fillId="4" -->
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="11"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <!-- fillId="5" -->
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="45"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <!-- fillId="6" -->
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="63"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <!-- fillId="7" -->
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="57"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <!-- fillId="8" -->
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="51"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <!-- fillId="9" -->
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="14"/>
@@ -276,6 +339,7 @@
     </fill>
   </fills>
   <borders count="33">
+    <!-- borderId="0" -->
     <border>
       <left/>
       <right/>
@@ -283,6 +347,7 @@
       <bottom/>
       <diagonal/>
     </border>
+    <!-- borderId="1" -->
     <border>
       <left style="thin">
         <color indexed="64"/>
@@ -296,6 +361,7 @@
       </bottom>
       <diagonal/>
     </border>
+    <!-- borderId="2" -->
     <border>
       <left/>
       <right/>
@@ -305,6 +371,7 @@
       <bottom/>
       <diagonal/>
     </border>
+    <!-- borderId="3" -->
     <border>
       <left/>
       <right style="thin">
@@ -318,6 +385,7 @@
       </bottom>
       <diagonal/>
     </border>
+    <!-- borderId="4" -->
     <border>
       <left style="thin">
         <color indexed="64"/>
@@ -329,6 +397,7 @@
       <bottom/>
       <diagonal/>
     </border>
+    <!-- borderId="5" -->
     <border>
       <left/>
       <right/>
@@ -338,6 +407,7 @@
       <bottom/>
       <diagonal/>
     </border>
+    <!-- borderId="6" -->
     <border>
       <left/>
       <right style="thin">
@@ -349,6 +419,7 @@
       <bottom/>
       <diagonal/>
     </border>
+    <!-- borderId="7" -->
     <border>
       <left style="thin">
         <color indexed="64"/>
@@ -362,6 +433,7 @@
       </bottom>
       <diagonal/>
     </border>
+    <!-- borderId="8" -->
     <border>
       <left style="thin">
         <color indexed="22"/>
@@ -375,6 +447,7 @@
       </bottom>
       <diagonal/>
     </border>
+    <!-- borderId="9" -->
     <border>
       <left style="thin">
         <color indexed="22"/>
@@ -388,6 +461,7 @@
       </bottom>
       <diagonal/>
     </border>
+    <!-- borderId="10" -->
     <border>
       <left style="thin">
         <color indexed="64"/>
@@ -403,6 +477,7 @@
       </bottom>
       <diagonal/>
     </border>
+    <!-- borderId="11" -->
     <border>
       <left style="thin">
         <color indexed="22"/>
@@ -418,6 +493,7 @@
       </bottom>
       <diagonal/>
     </border>
+    <!-- borderId="12" -->
     <border>
       <left style="thin">
         <color indexed="64"/>
@@ -431,6 +507,7 @@
       <bottom/>
       <diagonal/>
     </border>
+    <!-- borderId="13" -->
     <border>
       <left style="thin">
         <color indexed="22"/>
@@ -444,6 +521,7 @@
       <bottom/>
       <diagonal/>
     </border>
+    <!-- borderId="14" -->
     <border>
       <left style="thin">
         <color indexed="22"/>
@@ -455,6 +533,7 @@
       <bottom/>
       <diagonal/>
     </border>
+    <!-- borderId="15" -->
     <border>
       <left style="thin">
         <color indexed="64"/>
@@ -468,6 +547,7 @@
       </bottom>
       <diagonal/>
     </border>
+    <!-- borderId="16" -->
     <border>
       <left/>
       <right/>
@@ -479,6 +559,7 @@
       </bottom>
       <diagonal/>
     </border>
+    <!-- borderId="17" -->
     <border>
       <left style="medium">
         <color indexed="14"/>
@@ -494,6 +575,7 @@
       </bottom>
       <diagonal/>
     </border>
+    <!-- borderId="18" -->
     <border>
       <left style="thin">
         <color indexed="64"/>
@@ -505,6 +587,7 @@
       <bottom/>
       <diagonal/>
     </border>
+    <!-- borderId="19" -->
     <border>
       <left/>
       <right/>
@@ -514,6 +597,7 @@
       <bottom/>
       <diagonal/>
     </border>
+    <!-- borderId="20" -->
     <border>
       <left/>
       <right style="thin">
@@ -525,6 +609,7 @@
       <bottom/>
       <diagonal/>
     </border>
+    <!-- borderId="21" -->
     <border>
       <left style="thin">
         <color indexed="22"/>
@@ -538,6 +623,7 @@
       </bottom>
       <diagonal/>
     </border>
+    <!-- borderId="22" -->
     <border>
       <left style="thin">
         <color indexed="22"/>
@@ -551,6 +637,7 @@
       <bottom/>
       <diagonal/>
     </border>
+    <!-- borderId="23" -->
     <border>
       <left/>
       <right style="medium">
@@ -564,6 +651,7 @@
       </bottom>
       <diagonal/>
     </border>
+    <!-- borderId="24" -->
     <border>
       <left style="medium">
         <color indexed="14"/>
@@ -579,6 +667,7 @@
       </bottom>
       <diagonal/>
     </border>
+    <!-- borderId="25" -->
     <border>
       <left style="thin">
         <color indexed="64"/>
@@ -592,6 +681,7 @@
       </bottom>
       <diagonal/>
     </border>
+    <!-- borderId="26" -->
     <border>
       <left/>
       <right/>
@@ -603,6 +693,7 @@
       </bottom>
       <diagonal/>
     </border>
+    <!-- borderId="27" -->
     <border>
       <left style="medium">
         <color indexed="14"/>
@@ -618,6 +709,7 @@
       </bottom>
       <diagonal/>
     </border>
+    <!-- borderId="28" -->
     <border>
       <left style="medium">
         <color indexed="64"/>
@@ -631,6 +723,7 @@
       </bottom>
       <diagonal/>
     </border>
+    <!-- borderId="29" -->
     <border>
       <left style="thin">
         <color indexed="64"/>
@@ -640,6 +733,7 @@
       <bottom/>
       <diagonal/>
     </border>
+    <!-- borderId="30" -->
     <border>
       <left/>
       <right style="thin">
@@ -649,6 +743,7 @@
       <bottom/>
       <diagonal/>
     </border>
+    <!-- borderId="31" -->
     <border>
       <left style="thin">
         <color indexed="64"/>
@@ -660,6 +755,7 @@
       </bottom>
       <diagonal/>
     </border>
+    <!-- borderId="32" -->
     <border>
       <left/>
       <right/>
@@ -671,226 +767,305 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
+    <!-- cellStyleXfId="0" -->
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="77">
+    <!-- cellXfId="0" -->
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <!-- cellXfId="1" -->
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <!-- cellXfId="2" -->
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <!-- cellXfId="3" -->
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <!-- cellXfId="4" -->
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <!-- cellXfId="5" -->
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <!-- cellXfId="6" -->
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="7" -->
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <!-- cellXfId="8" -->
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <!-- cellXfId="9" -->
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <!-- cellXfId="10" -->
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <!-- cellXfId="11" -->
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <!-- cellXfId="12" -->
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <!-- cellXfId="13" -->
     <xf numFmtId="164" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="14" -->
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="15" -->
     <xf numFmtId="164" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="16" -->
     <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="17" -->
     <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="18" -->
     <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="19" -->
     <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="20" -->
     <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="21" -->
     <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="22" -->
     <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="23" -->
     <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="24" -->
     <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="25" -->
     <xf numFmtId="164" fontId="12" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="26" -->
     <xf numFmtId="164" fontId="12" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="27" -->
     <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="28" -->
     <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="29" -->
     <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="30" -->
     <xf numFmtId="164" fontId="12" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="31" -->
     <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="32" -->
     <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="33" -->
     <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="34" -->
     <xf numFmtId="164" fontId="12" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="35" -->
     <xf numFmtId="164" fontId="12" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="36" -->
     <xf numFmtId="0" fontId="12" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="37" -->
     <xf numFmtId="0" fontId="6" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="38" -->
     <xf numFmtId="0" fontId="6" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="39" -->
     <xf numFmtId="164" fontId="6" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="40" -->
     <xf numFmtId="164" fontId="12" fillId="5" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="41" -->
     <xf numFmtId="0" fontId="7" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="42" -->
     <xf numFmtId="0" fontId="6" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="43" -->
     <xf numFmtId="0" fontId="6" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="44" -->
     <xf numFmtId="0" fontId="6" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="45" -->
     <xf numFmtId="0" fontId="12" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="46" -->
     <xf numFmtId="0" fontId="12" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="47" -->
     <xf numFmtId="164" fontId="12" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="48" -->
     <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="49" -->
     <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="50" -->
     <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="51" -->
     <xf numFmtId="164" fontId="12" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="52" -->
     <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="53" -->
     <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="54" -->
     <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="55" -->
     <xf numFmtId="164" fontId="12" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="56" -->
     <xf numFmtId="164" fontId="12" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="57" -->
     <xf numFmtId="164" fontId="12" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="58" -->
     <xf numFmtId="164" fontId="12" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="59" -->
     <xf numFmtId="164" fontId="12" fillId="5" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="60" -->
     <xf numFmtId="0" fontId="12" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="61" -->
     <xf numFmtId="0" fontId="12" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="62" -->
     <xf numFmtId="0" fontId="12" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="63" -->
     <xf numFmtId="164" fontId="12" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="64" -->
     <xf numFmtId="164" fontId="12" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="65" -->
     <xf numFmtId="0" fontId="8" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="66" -->
     <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <!-- cellXfId="67" -->
     <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <!-- cellXfId="68" -->
     <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <!-- cellXfId="69" -->
     <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <!-- cellXfId="70" -->
     <xf numFmtId="0" fontId="10" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <!-- cellXfId="71" -->
     <xf numFmtId="0" fontId="4" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <!-- cellXfId="72" -->
     <xf numFmtId="0" fontId="9" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <!-- cellXfId="73" -->
     <xf numFmtId="0" fontId="8" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="74" -->
     <xf numFmtId="0" fontId="9" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <!-- cellXfId="75" -->
     <xf numFmtId="0" fontId="9" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <!-- cellXfId="76" -->
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
+    <!-- cellStyleId="0" -->
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>

</xml_diff>

<commit_message>
Added updates for latest PDFTronGo lib update. (#26)
Co-authored-by: jenkins <build@pdftron.com>
</commit_message>
<xml_diff>
--- a/samples/TestFiles/simple-excel_2007.xlsx
+++ b/samples/TestFiles/simple-excel_2007.xlsx
@@ -17,118 +17,157 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<!--OOXMLEditor: Added index comments-->
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+  <!-- String id="0" -->
   <si>
     <t>Quantity</t>
   </si>
+  <!-- String id="1" -->
   <si>
     <t>Total</t>
   </si>
+  <!-- String id="2" -->
   <si>
     <t>Soil</t>
   </si>
+  <!-- String id="3" -->
   <si>
     <t>Seeds</t>
   </si>
+  <!-- String id="4" -->
   <si>
     <t>Plants</t>
   </si>
+  <!-- String id="5" -->
   <si>
     <t>Flowers</t>
   </si>
+  <!-- String id="6" -->
   <si>
     <t>Trees</t>
   </si>
+  <!-- String id="7" -->
   <si>
     <t>Plant Food</t>
   </si>
+  <!-- String id="8" -->
   <si>
     <t>Mulch</t>
   </si>
+  <!-- String id="9" -->
   <si>
     <t>Total Costs</t>
   </si>
+  <!-- String id="10" -->
   <si>
     <t>Difference</t>
   </si>
+  <!-- String id="11" -->
   <si>
     <t>Fertilizer/Compost</t>
   </si>
+  <!-- String id="12" -->
   <si>
     <t>Description</t>
   </si>
+  <!-- String id="13" -->
   <si>
     <t>Name</t>
   </si>
+  <!-- String id="14" -->
   <si>
     <t>Total Plants</t>
   </si>
+  <!-- String id="15" -->
   <si>
     <t>Cost Each</t>
   </si>
+  <!-- String id="16" -->
   <si>
     <t>Total Flowers</t>
   </si>
+  <!-- String id="17" -->
   <si>
     <t>Total Trees</t>
   </si>
+  <!-- String id="18" -->
   <si>
     <t>Total Seeds</t>
   </si>
+  <!-- String id="19" -->
   <si>
     <t>Total Plant Food</t>
   </si>
+  <!-- String id="20" -->
   <si>
     <t>Total Soil</t>
   </si>
+  <!-- String id="21" -->
   <si>
     <t>Total Mulch</t>
   </si>
+  <!-- String id="22" -->
   <si>
     <t>Total Fertilizer/Compost</t>
   </si>
+  <!-- String id="23" -->
   <si>
     <t>Rhododendron</t>
   </si>
+  <!-- String id="24" -->
   <si>
     <t>Petunia</t>
   </si>
+  <!-- String id="25" -->
   <si>
     <t>Annual, purple and white</t>
   </si>
+  <!-- String id="26" -->
   <si>
     <t>Furniture/Statuary</t>
   </si>
+  <!-- String id="27" -->
   <si>
     <t>Total Furniture/Statuary</t>
   </si>
+  <!-- String id="28" -->
   <si>
     <t>Fencing</t>
   </si>
+  <!-- String id="29" -->
   <si>
     <t>Total Fencing</t>
   </si>
+  <!-- String id="30" -->
   <si>
     <t>Japanese Maple</t>
   </si>
+  <!-- String id="31" -->
   <si>
     <t>Leafy tree</t>
   </si>
+  <!-- String id="32" -->
   <si>
     <t>Herbicides/Pesticides</t>
   </si>
+  <!-- String id="33" -->
   <si>
     <t>Total Herbicides/Pesticides</t>
   </si>
+  <!-- String id="34" -->
   <si>
     <t>Flowering evergreen</t>
   </si>
+  <!-- String id="35" -->
   <si>
     <t xml:space="preserve">   </t>
   </si>
+  <!-- String id="36" -->
   <si>
     <t>Budgeted amount</t>
   </si>
+  <!-- String id="37" -->
   <si>
     <t xml:space="preserve"> Garden Budget</t>
   </si>
@@ -136,21 +175,25 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
+<!--OOXMLEditor: Added index comments-->
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="13">
+    <!-- fontId="0" -->
     <font>
       <sz val="10"/>
       <name val="Arial"/>
     </font>
+    <!-- fontId="1" -->
     <font>
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <!-- fontId="2" -->
     <font>
       <b/>
       <sz val="9"/>
@@ -158,11 +201,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <!-- fontId="3" -->
     <font>
       <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <!-- fontId="4" -->
     <font>
       <b/>
       <sz val="24"/>
@@ -170,6 +215,7 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <!-- fontId="5" -->
     <font>
       <b/>
       <sz val="26"/>
@@ -177,97 +223,114 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <!-- fontId="6" -->
     <font>
       <sz val="10"/>
-      <name val="Century Gothic"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
+    <!-- fontId="7" -->
     <font>
       <b/>
       <sz val="10"/>
-      <name val="Century Gothic"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
+    <!-- fontId="8" -->
     <font>
       <b/>
       <sz val="10"/>
       <color indexed="9"/>
-      <name val="Century Gothic"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
+    <!-- fontId="9" -->
     <font>
       <sz val="10"/>
       <color indexed="9"/>
-      <name val="Century Gothic"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
+    <!-- fontId="10" -->
     <font>
       <sz val="9"/>
       <color indexed="9"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <!-- fontId="11" -->
     <font>
       <sz val="22"/>
       <color indexed="9"/>
-      <name val="Century Gothic"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
+    <!-- fontId="12" -->
     <font>
       <sz val="9"/>
-      <name val="Century Gothic"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
   <fills count="10">
+    <!-- fillId="0" -->
     <fill>
       <patternFill patternType="none"/>
     </fill>
+    <!-- fillId="1" -->
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <!-- fillId="2" -->
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="14"/>
         <bgColor indexed="24"/>
       </patternFill>
     </fill>
+    <!-- fillId="3" -->
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="63"/>
         <bgColor indexed="24"/>
       </patternFill>
     </fill>
+    <!-- fillId="4" -->
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="11"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <!-- fillId="5" -->
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="45"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <!-- fillId="6" -->
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="63"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <!-- fillId="7" -->
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="57"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <!-- fillId="8" -->
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="51"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <!-- fillId="9" -->
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="14"/>
@@ -276,6 +339,7 @@
     </fill>
   </fills>
   <borders count="33">
+    <!-- borderId="0" -->
     <border>
       <left/>
       <right/>
@@ -283,6 +347,7 @@
       <bottom/>
       <diagonal/>
     </border>
+    <!-- borderId="1" -->
     <border>
       <left style="thin">
         <color indexed="64"/>
@@ -296,6 +361,7 @@
       </bottom>
       <diagonal/>
     </border>
+    <!-- borderId="2" -->
     <border>
       <left/>
       <right/>
@@ -305,6 +371,7 @@
       <bottom/>
       <diagonal/>
     </border>
+    <!-- borderId="3" -->
     <border>
       <left/>
       <right style="thin">
@@ -318,6 +385,7 @@
       </bottom>
       <diagonal/>
     </border>
+    <!-- borderId="4" -->
     <border>
       <left style="thin">
         <color indexed="64"/>
@@ -329,6 +397,7 @@
       <bottom/>
       <diagonal/>
     </border>
+    <!-- borderId="5" -->
     <border>
       <left/>
       <right/>
@@ -338,6 +407,7 @@
       <bottom/>
       <diagonal/>
     </border>
+    <!-- borderId="6" -->
     <border>
       <left/>
       <right style="thin">
@@ -349,6 +419,7 @@
       <bottom/>
       <diagonal/>
     </border>
+    <!-- borderId="7" -->
     <border>
       <left style="thin">
         <color indexed="64"/>
@@ -362,6 +433,7 @@
       </bottom>
       <diagonal/>
     </border>
+    <!-- borderId="8" -->
     <border>
       <left style="thin">
         <color indexed="22"/>
@@ -375,6 +447,7 @@
       </bottom>
       <diagonal/>
     </border>
+    <!-- borderId="9" -->
     <border>
       <left style="thin">
         <color indexed="22"/>
@@ -388,6 +461,7 @@
       </bottom>
       <diagonal/>
     </border>
+    <!-- borderId="10" -->
     <border>
       <left style="thin">
         <color indexed="64"/>
@@ -403,6 +477,7 @@
       </bottom>
       <diagonal/>
     </border>
+    <!-- borderId="11" -->
     <border>
       <left style="thin">
         <color indexed="22"/>
@@ -418,6 +493,7 @@
       </bottom>
       <diagonal/>
     </border>
+    <!-- borderId="12" -->
     <border>
       <left style="thin">
         <color indexed="64"/>
@@ -431,6 +507,7 @@
       <bottom/>
       <diagonal/>
     </border>
+    <!-- borderId="13" -->
     <border>
       <left style="thin">
         <color indexed="22"/>
@@ -444,6 +521,7 @@
       <bottom/>
       <diagonal/>
     </border>
+    <!-- borderId="14" -->
     <border>
       <left style="thin">
         <color indexed="22"/>
@@ -455,6 +533,7 @@
       <bottom/>
       <diagonal/>
     </border>
+    <!-- borderId="15" -->
     <border>
       <left style="thin">
         <color indexed="64"/>
@@ -468,6 +547,7 @@
       </bottom>
       <diagonal/>
     </border>
+    <!-- borderId="16" -->
     <border>
       <left/>
       <right/>
@@ -479,6 +559,7 @@
       </bottom>
       <diagonal/>
     </border>
+    <!-- borderId="17" -->
     <border>
       <left style="medium">
         <color indexed="14"/>
@@ -494,6 +575,7 @@
       </bottom>
       <diagonal/>
     </border>
+    <!-- borderId="18" -->
     <border>
       <left style="thin">
         <color indexed="64"/>
@@ -505,6 +587,7 @@
       <bottom/>
       <diagonal/>
     </border>
+    <!-- borderId="19" -->
     <border>
       <left/>
       <right/>
@@ -514,6 +597,7 @@
       <bottom/>
       <diagonal/>
     </border>
+    <!-- borderId="20" -->
     <border>
       <left/>
       <right style="thin">
@@ -525,6 +609,7 @@
       <bottom/>
       <diagonal/>
     </border>
+    <!-- borderId="21" -->
     <border>
       <left style="thin">
         <color indexed="22"/>
@@ -538,6 +623,7 @@
       </bottom>
       <diagonal/>
     </border>
+    <!-- borderId="22" -->
     <border>
       <left style="thin">
         <color indexed="22"/>
@@ -551,6 +637,7 @@
       <bottom/>
       <diagonal/>
     </border>
+    <!-- borderId="23" -->
     <border>
       <left/>
       <right style="medium">
@@ -564,6 +651,7 @@
       </bottom>
       <diagonal/>
     </border>
+    <!-- borderId="24" -->
     <border>
       <left style="medium">
         <color indexed="14"/>
@@ -579,6 +667,7 @@
       </bottom>
       <diagonal/>
     </border>
+    <!-- borderId="25" -->
     <border>
       <left style="thin">
         <color indexed="64"/>
@@ -592,6 +681,7 @@
       </bottom>
       <diagonal/>
     </border>
+    <!-- borderId="26" -->
     <border>
       <left/>
       <right/>
@@ -603,6 +693,7 @@
       </bottom>
       <diagonal/>
     </border>
+    <!-- borderId="27" -->
     <border>
       <left style="medium">
         <color indexed="14"/>
@@ -618,6 +709,7 @@
       </bottom>
       <diagonal/>
     </border>
+    <!-- borderId="28" -->
     <border>
       <left style="medium">
         <color indexed="64"/>
@@ -631,6 +723,7 @@
       </bottom>
       <diagonal/>
     </border>
+    <!-- borderId="29" -->
     <border>
       <left style="thin">
         <color indexed="64"/>
@@ -640,6 +733,7 @@
       <bottom/>
       <diagonal/>
     </border>
+    <!-- borderId="30" -->
     <border>
       <left/>
       <right style="thin">
@@ -649,6 +743,7 @@
       <bottom/>
       <diagonal/>
     </border>
+    <!-- borderId="31" -->
     <border>
       <left style="thin">
         <color indexed="64"/>
@@ -660,6 +755,7 @@
       </bottom>
       <diagonal/>
     </border>
+    <!-- borderId="32" -->
     <border>
       <left/>
       <right/>
@@ -671,226 +767,305 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
+    <!-- cellStyleXfId="0" -->
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="77">
+    <!-- cellXfId="0" -->
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <!-- cellXfId="1" -->
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <!-- cellXfId="2" -->
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <!-- cellXfId="3" -->
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <!-- cellXfId="4" -->
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <!-- cellXfId="5" -->
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <!-- cellXfId="6" -->
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="7" -->
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <!-- cellXfId="8" -->
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <!-- cellXfId="9" -->
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <!-- cellXfId="10" -->
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <!-- cellXfId="11" -->
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <!-- cellXfId="12" -->
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <!-- cellXfId="13" -->
     <xf numFmtId="164" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="14" -->
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="15" -->
     <xf numFmtId="164" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="16" -->
     <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="17" -->
     <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="18" -->
     <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="19" -->
     <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="20" -->
     <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="21" -->
     <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="22" -->
     <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="23" -->
     <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="24" -->
     <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="25" -->
     <xf numFmtId="164" fontId="12" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="26" -->
     <xf numFmtId="164" fontId="12" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="27" -->
     <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="28" -->
     <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="29" -->
     <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="30" -->
     <xf numFmtId="164" fontId="12" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="31" -->
     <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="32" -->
     <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="33" -->
     <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="34" -->
     <xf numFmtId="164" fontId="12" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="35" -->
     <xf numFmtId="164" fontId="12" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="36" -->
     <xf numFmtId="0" fontId="12" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="37" -->
     <xf numFmtId="0" fontId="6" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="38" -->
     <xf numFmtId="0" fontId="6" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="39" -->
     <xf numFmtId="164" fontId="6" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="40" -->
     <xf numFmtId="164" fontId="12" fillId="5" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="41" -->
     <xf numFmtId="0" fontId="7" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="42" -->
     <xf numFmtId="0" fontId="6" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="43" -->
     <xf numFmtId="0" fontId="6" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="44" -->
     <xf numFmtId="0" fontId="6" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="45" -->
     <xf numFmtId="0" fontId="12" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="46" -->
     <xf numFmtId="0" fontId="12" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="47" -->
     <xf numFmtId="164" fontId="12" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="48" -->
     <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="49" -->
     <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="50" -->
     <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="51" -->
     <xf numFmtId="164" fontId="12" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="52" -->
     <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="53" -->
     <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="54" -->
     <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="55" -->
     <xf numFmtId="164" fontId="12" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="56" -->
     <xf numFmtId="164" fontId="12" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="57" -->
     <xf numFmtId="164" fontId="12" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="58" -->
     <xf numFmtId="164" fontId="12" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="59" -->
     <xf numFmtId="164" fontId="12" fillId="5" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="60" -->
     <xf numFmtId="0" fontId="12" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="61" -->
     <xf numFmtId="0" fontId="12" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="62" -->
     <xf numFmtId="0" fontId="12" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="63" -->
     <xf numFmtId="164" fontId="12" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="64" -->
     <xf numFmtId="164" fontId="12" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="65" -->
     <xf numFmtId="0" fontId="8" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="66" -->
     <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <!-- cellXfId="67" -->
     <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <!-- cellXfId="68" -->
     <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <!-- cellXfId="69" -->
     <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <!-- cellXfId="70" -->
     <xf numFmtId="0" fontId="10" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <!-- cellXfId="71" -->
     <xf numFmtId="0" fontId="4" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <!-- cellXfId="72" -->
     <xf numFmtId="0" fontId="9" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <!-- cellXfId="73" -->
     <xf numFmtId="0" fontId="8" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <!-- cellXfId="74" -->
     <xf numFmtId="0" fontId="9" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <!-- cellXfId="75" -->
     <xf numFmtId="0" fontId="9" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <!-- cellXfId="76" -->
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
+    <!-- cellStyleId="0" -->
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>

</xml_diff>